<commit_message>
Updated to best current data, finished tendon model fitting code, initial hopper simulation scripts
</commit_message>
<xml_diff>
--- a/data/sampledata.xlsx
+++ b/data/sampledata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="0" windowWidth="17880" windowHeight="12180" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="3960" yWindow="0" windowWidth="17880" windowHeight="12180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -559,24 +559,24 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>16.739999999999998</v>
+        <v>17.309999999999999</v>
       </c>
       <c r="D3">
-        <v>0.93</v>
+        <v>1.58</v>
       </c>
       <c r="E3">
-        <v>3.06</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="F3">
         <f>B3/($A$20*C3)</f>
-        <v>3.0935313193377711E-3</v>
+        <v>2.0632169678963443E-3</v>
       </c>
       <c r="G3">
         <f>(PI()/4)*D3*E3</f>
-        <v>2.2350860933964585</v>
+        <v>1.3898405899481248</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -601,7 +601,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G5">
-        <v>492</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -637,46 +638,37 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>96.65</v>
+        <v>103.23</v>
       </c>
       <c r="C9">
-        <v>17.440000000000001</v>
+        <v>15.57</v>
       </c>
       <c r="D9">
-        <v>1.24</v>
+        <v>3.6</v>
+      </c>
+      <c r="E9">
+        <v>1.05</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>4.9480873197903013E-3</v>
+        <v>5.9196944673823287E-3</v>
       </c>
       <c r="G9">
         <f>(PI()/4)*D9*E9</f>
-        <v>0</v>
+        <v>2.9688050576423546</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10">
-        <v>100</v>
-      </c>
-      <c r="C10">
-        <v>17.98</v>
-      </c>
-      <c r="D10">
-        <v>2.44</v>
-      </c>
-      <c r="E10">
-        <v>3.28</v>
-      </c>
-      <c r="F10">
+      <c r="F10" t="e">
         <f t="shared" si="0"/>
-        <v>4.9658350548228182E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:G11" si="2">(PI()/4)*D10*E10</f>
-        <v>6.2856985813024577</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -722,24 +714,24 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <v>66.12</v>
+        <v>65</v>
       </c>
       <c r="C15">
-        <v>17.309999999999999</v>
+        <v>20.74</v>
       </c>
       <c r="D15">
-        <v>2.82</v>
+        <v>3.91</v>
       </c>
       <c r="E15">
-        <v>1.44</v>
+        <v>0.75</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>3.4104976479326574E-3</v>
+        <v>2.7982504477200719E-3</v>
       </c>
       <c r="G15">
         <f>(PI()/4)*D15*E15</f>
-        <v>3.1893448619243578</v>
+        <v>2.303180114163017</v>
       </c>
       <c r="H15" s="2"/>
     </row>

</xml_diff>

<commit_message>
Final testing data added and processed, OpenSim plots updated
</commit_message>
<xml_diff>
--- a/data/sampledata.xlsx
+++ b/data/sampledata.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="3960" yWindow="0" windowWidth="17880" windowHeight="12180" tabRatio="500"/>
+    <workbookView xWindow="6600" yWindow="0" windowWidth="17880" windowHeight="12180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -583,26 +583,50 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="e">
+      <c r="B4">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D4">
+        <v>4.01</v>
+      </c>
+      <c r="E4">
+        <v>1.2</v>
+      </c>
+      <c r="F4">
         <f t="shared" ref="F4:F17" si="0">B4/($A$20*C4)</f>
-        <v>#DIV/0!</v>
+        <v>5.0379090183559454E-3</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G5" si="1">(PI()/4)*D4*E4</f>
-        <v>0</v>
+        <v>3.779335962268521</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="e">
+      <c r="B5">
+        <v>72</v>
+      </c>
+      <c r="C5">
+        <v>17.97</v>
+      </c>
+      <c r="D5">
+        <v>3.34</v>
+      </c>
+      <c r="E5">
+        <v>1.23</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.5773908895778681E-3</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.2265727348693969</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -662,26 +686,50 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" t="e">
+      <c r="B10">
+        <v>72</v>
+      </c>
+      <c r="C10">
+        <v>19.329999999999998</v>
+      </c>
+      <c r="D10">
+        <v>3.75</v>
+      </c>
+      <c r="E10">
+        <v>1.2</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.3256965486660262E-3</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:G11" si="2">(PI()/4)*D10*E10</f>
-        <v>0</v>
+        <v>3.5342917352885168</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="F11" t="e">
+      <c r="B11">
+        <v>76</v>
+      </c>
+      <c r="C11">
+        <v>18.39</v>
+      </c>
+      <c r="D11">
+        <v>3.56</v>
+      </c>
+      <c r="E11">
+        <v>0.73</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.6898935757010798E-3</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.0410927470372888</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -739,13 +787,25 @@
       <c r="A16" t="s">
         <v>1</v>
       </c>
-      <c r="F16" t="e">
+      <c r="B16">
+        <v>121</v>
+      </c>
+      <c r="C16">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="D16">
+        <v>3.97</v>
+      </c>
+      <c r="E16">
+        <v>1.51</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>5.7649794175941458E-3</v>
       </c>
       <c r="G16">
         <f>(PI()/4)*D16*E16</f>
-        <v>0</v>
+        <v>4.7082263701186831</v>
       </c>
       <c r="H16" s="2"/>
     </row>
@@ -753,13 +813,25 @@
       <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="F17" t="e">
+      <c r="B17">
+        <v>138</v>
+      </c>
+      <c r="C17">
+        <v>18.55</v>
+      </c>
+      <c r="D17">
+        <v>4.3</v>
+      </c>
+      <c r="E17">
+        <v>1.73</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>6.6422795533307667E-3</v>
       </c>
       <c r="G17">
         <f>(PI()/4)*D17*E17</f>
-        <v>0</v>
+        <v>5.8425769375136181</v>
       </c>
       <c r="H17" s="2"/>
     </row>

</xml_diff>